<commit_message>
Parte 1 y 2 ordenada, faltan bodes y gráficos. A hacer a continuación
</commit_message>
<xml_diff>
--- a/TP1/Mediciones/Mediciones.xlsx
+++ b/TP1/Mediciones/Mediciones.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\germa\Documents\GitHub\LABO\TP1\Mediciones\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{426DEF3F-2831-4D1A-88D6-DD135F812030}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF2D7256-0B91-459C-A3E2-6E9F61AD11E6}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{555DA7CC-7A38-4795-B3ED-2A85C07D66EC}"/>
   </bookViews>
@@ -31,28 +31,6 @@
     </ext>
   </extLst>
 </workbook>
-</file>
-
-<file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
-  <metadataTypes count="1">
-    <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
-  </metadataTypes>
-  <futureMetadata name="XLDAPR" count="1">
-    <bk>
-      <extLst>
-        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
-          <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
-        </ext>
-      </extLst>
-    </bk>
-  </futureMetadata>
-  <cellMetadata count="1">
-    <bk>
-      <rc t="1" v="0"/>
-    </bk>
-  </cellMetadata>
-</metadata>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
@@ -816,8 +794,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8E176629-7EB4-41C6-8CEB-BD43773D0D56}">
   <dimension ref="A1:S28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="O28" sqref="O28"/>
+    <sheetView tabSelected="1" topLeftCell="E10" workbookViewId="0">
+      <selection activeCell="O29" sqref="O29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1016,7 +994,7 @@
         <v>30</v>
       </c>
       <c r="P5" s="16">
-        <f t="shared" ref="P5:P27" si="3">ASIN(R5/S5)*(180/PI())</f>
+        <f t="shared" ref="P5:P28" si="3">ASIN(R5/S5)*(180/PI())</f>
         <v>1.2382926514488748</v>
       </c>
       <c r="Q5">
@@ -1921,12 +1899,15 @@
       </c>
       <c r="P26" s="16">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>78.410659015772893</v>
       </c>
       <c r="Q26">
         <f t="shared" si="2"/>
         <v>9</v>
       </c>
+      <c r="R26">
+        <v>9.61</v>
+      </c>
       <c r="S26" s="1">
         <v>9.81</v>
       </c>
@@ -1957,12 +1938,15 @@
       </c>
       <c r="P27" s="16">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>78.410659015772893</v>
       </c>
       <c r="Q27">
         <f t="shared" si="2"/>
         <v>9.25</v>
       </c>
+      <c r="R27">
+        <v>9.61</v>
+      </c>
       <c r="S27" s="1">
         <v>9.81</v>
       </c>
@@ -1991,13 +1975,16 @@
       <c r="O28" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="P28" s="16" t="e" cm="1">
-        <f t="array" aca="1" ref="P28" ca="1">aseno(R28/S28)</f>
-        <v>#NAME?</v>
+      <c r="P28" s="16">
+        <f t="shared" si="3"/>
+        <v>78.410659015772893</v>
       </c>
       <c r="Q28">
         <f t="shared" si="2"/>
         <v>9.51</v>
+      </c>
+      <c r="R28">
+        <v>9.61</v>
       </c>
       <c r="S28" s="1">
         <v>9.81</v>
@@ -2028,7 +2015,7 @@
   <dimension ref="A1:H23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H6" sqref="H6"/>
+      <selection activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>